<commit_message>
added 6 more rows
</commit_message>
<xml_diff>
--- a/aerobe_lab_data.xlsx
+++ b/aerobe_lab_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,6 +531,54 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>